<commit_message>
fixed Rscape + nonmp version
</commit_message>
<xml_diff>
--- a/benchmarks/summary.xlsx
+++ b/benchmarks/summary.xlsx
@@ -292,7 +292,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -417,7 +417,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -425,15 +433,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -441,15 +449,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -457,83 +465,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -569,9 +513,9 @@
   <dimension ref="A1:AMJ63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L37" activeCellId="0" sqref="L37"/>
+      <selection pane="bottomLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1309,7 +1253,7 @@
         <f aca="false">ROUND(2*J17*J20/(J17+J20),3)</f>
         <v>0.69</v>
       </c>
-      <c r="K14" s="31" t="n">
+      <c r="K14" s="13" t="n">
         <f aca="false">ROUND(2*K17*K20/(K17+K20),3)</f>
         <v>0.818</v>
       </c>
@@ -1342,43 +1286,43 @@
       <c r="C15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="32" t="n">
+      <c r="D15" s="17" t="n">
         <v>0.739</v>
       </c>
-      <c r="E15" s="32" t="n">
+      <c r="E15" s="17" t="n">
         <v>0.757</v>
       </c>
-      <c r="F15" s="32" t="n">
+      <c r="F15" s="17" t="n">
         <v>0.815</v>
       </c>
-      <c r="G15" s="33" t="n">
+      <c r="G15" s="18" t="n">
         <v>0.846</v>
       </c>
-      <c r="H15" s="34" t="n">
+      <c r="H15" s="19" t="n">
         <v>0.733</v>
       </c>
-      <c r="I15" s="32" t="n">
+      <c r="I15" s="17" t="n">
         <v>0.725</v>
       </c>
-      <c r="J15" s="32" t="n">
+      <c r="J15" s="17" t="n">
         <v>0.726</v>
       </c>
-      <c r="K15" s="34" t="n">
+      <c r="K15" s="19" t="n">
         <v>0.793</v>
       </c>
-      <c r="L15" s="32" t="n">
+      <c r="L15" s="17" t="n">
         <v>0.771</v>
       </c>
-      <c r="M15" s="35" t="n">
+      <c r="M15" s="16" t="n">
         <v>0.726</v>
       </c>
-      <c r="N15" s="32" t="n">
+      <c r="N15" s="17" t="n">
         <v>0.844</v>
       </c>
-      <c r="O15" s="32" t="n">
+      <c r="O15" s="17" t="n">
         <v>0.815</v>
       </c>
-      <c r="P15" s="35" t="n">
+      <c r="P15" s="16" t="n">
         <v>0.726</v>
       </c>
     </row>
@@ -1388,43 +1332,43 @@
       <c r="C16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="36" t="n">
+      <c r="D16" s="20" t="n">
         <v>0.719</v>
       </c>
-      <c r="E16" s="36" t="n">
+      <c r="E16" s="20" t="n">
         <v>0.759</v>
       </c>
-      <c r="F16" s="36" t="n">
+      <c r="F16" s="20" t="n">
         <v>0.818</v>
       </c>
-      <c r="G16" s="37" t="n">
+      <c r="G16" s="21" t="n">
         <v>0.891</v>
       </c>
-      <c r="H16" s="38" t="n">
+      <c r="H16" s="22" t="n">
         <v>0.716</v>
       </c>
-      <c r="I16" s="36" t="n">
+      <c r="I16" s="20" t="n">
         <v>0.703</v>
       </c>
-      <c r="J16" s="36" t="n">
+      <c r="J16" s="20" t="n">
         <v>0.775</v>
       </c>
-      <c r="K16" s="38" t="n">
+      <c r="K16" s="22" t="n">
         <v>0.787</v>
       </c>
-      <c r="L16" s="36" t="n">
+      <c r="L16" s="20" t="n">
         <v>0.756</v>
       </c>
-      <c r="M16" s="39" t="n">
+      <c r="M16" s="10" t="n">
         <v>0.775</v>
       </c>
-      <c r="N16" s="36" t="n">
+      <c r="N16" s="20" t="n">
         <v>0.845</v>
       </c>
-      <c r="O16" s="36" t="n">
+      <c r="O16" s="20" t="n">
         <v>0.807</v>
       </c>
-      <c r="P16" s="39" t="n">
+      <c r="P16" s="10" t="n">
         <v>0.775</v>
       </c>
     </row>
@@ -1434,43 +1378,43 @@
       <c r="C17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="40" t="n">
+      <c r="D17" s="23" t="n">
         <v>0.76</v>
       </c>
-      <c r="E17" s="40" t="n">
+      <c r="E17" s="23" t="n">
         <v>0.754</v>
       </c>
-      <c r="F17" s="41" t="n">
+      <c r="F17" s="24" t="n">
         <v>0.812</v>
       </c>
-      <c r="G17" s="40" t="n">
+      <c r="G17" s="23" t="n">
         <v>0.805</v>
       </c>
-      <c r="H17" s="42" t="n">
+      <c r="H17" s="25" t="n">
         <v>0.751</v>
       </c>
-      <c r="I17" s="40" t="n">
+      <c r="I17" s="23" t="n">
         <v>0.747</v>
       </c>
-      <c r="J17" s="40" t="n">
+      <c r="J17" s="23" t="n">
         <v>0.683</v>
       </c>
-      <c r="K17" s="42" t="n">
+      <c r="K17" s="25" t="n">
         <v>0.798</v>
       </c>
-      <c r="L17" s="40" t="n">
+      <c r="L17" s="23" t="n">
         <v>0.786</v>
       </c>
-      <c r="M17" s="43" t="n">
+      <c r="M17" s="8" t="n">
         <v>0.683</v>
       </c>
-      <c r="N17" s="40" t="n">
+      <c r="N17" s="23" t="n">
         <v>0.844</v>
       </c>
-      <c r="O17" s="40" t="n">
+      <c r="O17" s="23" t="n">
         <v>0.824</v>
       </c>
-      <c r="P17" s="43" t="n">
+      <c r="P17" s="8" t="n">
         <v>0.683</v>
       </c>
     </row>
@@ -1482,43 +1426,43 @@
       <c r="C18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="36" t="n">
+      <c r="D18" s="20" t="n">
         <v>0.743</v>
       </c>
-      <c r="E18" s="36" t="n">
+      <c r="E18" s="20" t="n">
         <v>0.756</v>
       </c>
-      <c r="F18" s="36" t="n">
+      <c r="F18" s="20" t="n">
         <v>0.813</v>
       </c>
-      <c r="G18" s="37" t="n">
+      <c r="G18" s="21" t="n">
         <v>0.847</v>
       </c>
-      <c r="H18" s="38" t="n">
+      <c r="H18" s="22" t="n">
         <v>0.735</v>
       </c>
-      <c r="I18" s="36" t="n">
+      <c r="I18" s="20" t="n">
         <v>0.731</v>
       </c>
-      <c r="J18" s="36" t="n">
+      <c r="J18" s="20" t="n">
         <v>0.717</v>
       </c>
-      <c r="K18" s="38" t="n">
+      <c r="K18" s="22" t="n">
         <v>0.814</v>
       </c>
-      <c r="L18" s="36" t="n">
+      <c r="L18" s="20" t="n">
         <v>0.791</v>
       </c>
-      <c r="M18" s="39" t="n">
+      <c r="M18" s="10" t="n">
         <v>0.717</v>
       </c>
-      <c r="N18" s="36" t="n">
+      <c r="N18" s="20" t="n">
         <v>0.856</v>
       </c>
-      <c r="O18" s="36" t="n">
+      <c r="O18" s="20" t="n">
         <v>0.82</v>
       </c>
-      <c r="P18" s="39" t="n">
+      <c r="P18" s="10" t="n">
         <v>0.717</v>
       </c>
     </row>
@@ -1528,43 +1472,43 @@
       <c r="C19" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="36" t="n">
+      <c r="D19" s="20" t="n">
         <v>0.731</v>
       </c>
-      <c r="E19" s="36" t="n">
+      <c r="E19" s="20" t="n">
         <v>0.765</v>
       </c>
-      <c r="F19" s="36" t="n">
+      <c r="F19" s="20" t="n">
         <v>0.811</v>
       </c>
-      <c r="G19" s="37" t="n">
+      <c r="G19" s="21" t="n">
         <v>0.883</v>
       </c>
-      <c r="H19" s="38" t="n">
+      <c r="H19" s="22" t="n">
         <v>0.719</v>
       </c>
-      <c r="I19" s="36" t="n">
+      <c r="I19" s="20" t="n">
         <v>0.714</v>
       </c>
-      <c r="J19" s="36" t="n">
+      <c r="J19" s="20" t="n">
         <v>0.766</v>
       </c>
-      <c r="K19" s="38" t="n">
+      <c r="K19" s="22" t="n">
         <v>0.81</v>
       </c>
-      <c r="L19" s="36" t="n">
+      <c r="L19" s="20" t="n">
         <v>0.778</v>
       </c>
-      <c r="M19" s="39" t="n">
+      <c r="M19" s="10" t="n">
         <v>0.766</v>
       </c>
-      <c r="N19" s="36" t="n">
+      <c r="N19" s="20" t="n">
         <v>0.862</v>
       </c>
-      <c r="O19" s="36" t="n">
+      <c r="O19" s="20" t="n">
         <v>0.819</v>
       </c>
-      <c r="P19" s="39" t="n">
+      <c r="P19" s="10" t="n">
         <v>0.766</v>
       </c>
     </row>
@@ -1574,43 +1518,43 @@
       <c r="C20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="36" t="n">
+      <c r="D20" s="20" t="n">
         <v>0.767</v>
       </c>
-      <c r="E20" s="36" t="n">
+      <c r="E20" s="20" t="n">
         <v>0.762</v>
       </c>
-      <c r="F20" s="36" t="n">
+      <c r="F20" s="20" t="n">
         <v>0.83</v>
       </c>
-      <c r="G20" s="36" t="n">
+      <c r="G20" s="20" t="n">
         <v>0.834</v>
       </c>
-      <c r="H20" s="38" t="n">
+      <c r="H20" s="22" t="n">
         <v>0.768</v>
       </c>
-      <c r="I20" s="36" t="n">
+      <c r="I20" s="20" t="n">
         <v>0.768</v>
       </c>
-      <c r="J20" s="36" t="n">
+      <c r="J20" s="20" t="n">
         <v>0.698</v>
       </c>
-      <c r="K20" s="44" t="n">
+      <c r="K20" s="26" t="n">
         <v>0.84</v>
       </c>
-      <c r="L20" s="36" t="n">
+      <c r="L20" s="20" t="n">
         <v>0.82</v>
       </c>
-      <c r="M20" s="39" t="n">
+      <c r="M20" s="10" t="n">
         <v>0.698</v>
       </c>
-      <c r="N20" s="36" t="n">
+      <c r="N20" s="20" t="n">
         <v>0.87</v>
       </c>
-      <c r="O20" s="36" t="n">
+      <c r="O20" s="20" t="n">
         <v>0.844</v>
       </c>
-      <c r="P20" s="39" t="n">
+      <c r="P20" s="10" t="n">
         <v>0.698</v>
       </c>
     </row>
@@ -1620,43 +1564,43 @@
         <v>23</v>
       </c>
       <c r="C21" s="27"/>
-      <c r="D21" s="45" t="n">
+      <c r="D21" s="28" t="n">
         <v>0.3</v>
       </c>
-      <c r="E21" s="45" t="n">
+      <c r="E21" s="28" t="n">
         <v>1.9</v>
       </c>
-      <c r="F21" s="45" t="n">
+      <c r="F21" s="28" t="n">
         <v>25.5</v>
       </c>
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="46" t="n">
+      <c r="H21" s="29" t="n">
         <v>24.7</v>
       </c>
-      <c r="I21" s="45" t="n">
+      <c r="I21" s="28" t="n">
         <v>12.3</v>
       </c>
-      <c r="J21" s="45" t="n">
+      <c r="J21" s="28" t="n">
         <v>7.8</v>
       </c>
-      <c r="K21" s="46" t="n">
+      <c r="K21" s="29" t="n">
         <v>24.7</v>
       </c>
-      <c r="L21" s="45" t="n">
+      <c r="L21" s="28" t="n">
         <v>12.3</v>
       </c>
-      <c r="M21" s="47" t="n">
+      <c r="M21" s="30" t="n">
         <v>7.8</v>
       </c>
-      <c r="N21" s="45" t="n">
+      <c r="N21" s="28" t="n">
         <v>25.9</v>
       </c>
-      <c r="O21" s="45" t="n">
+      <c r="O21" s="28" t="n">
         <v>12.6</v>
       </c>
-      <c r="P21" s="47" t="n">
+      <c r="P21" s="30" t="n">
         <v>7.8</v>
       </c>
     </row>
@@ -1698,7 +1642,7 @@
         <f aca="false">ROUND(2*J25*J28/(J25+J28),3)</f>
         <v>0.716</v>
       </c>
-      <c r="K22" s="48" t="n">
+      <c r="K22" s="31" t="n">
         <f aca="false">ROUND(2*K25*K28/(K25+K28),3)</f>
         <v>0.854</v>
       </c>
@@ -1757,7 +1701,7 @@
         <f aca="false">ROUND(2*J26*J29/(J26+J29),3)</f>
         <v>0.823</v>
       </c>
-      <c r="K23" s="48" t="n">
+      <c r="K23" s="31" t="n">
         <f aca="false">ROUND(2*K26*K29/(K26+K29),3)</f>
         <v>0.852</v>
       </c>
@@ -1816,7 +1760,7 @@
         <f aca="false">ROUND(2*J27*J30/(J27+J30),3)</f>
         <v>0.673</v>
       </c>
-      <c r="K24" s="48" t="n">
+      <c r="K24" s="31" t="n">
         <f aca="false">ROUND(2*K27*K30/(K27+K30),3)</f>
         <v>0.866</v>
       </c>
@@ -1849,43 +1793,43 @@
       <c r="C25" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="32" t="n">
+      <c r="D25" s="17" t="n">
         <v>0.772</v>
       </c>
-      <c r="E25" s="32" t="n">
+      <c r="E25" s="17" t="n">
         <v>0.779</v>
       </c>
-      <c r="F25" s="32" t="n">
+      <c r="F25" s="17" t="n">
         <v>0.822</v>
       </c>
-      <c r="G25" s="32" t="n">
+      <c r="G25" s="17" t="n">
         <v>0.843</v>
       </c>
-      <c r="H25" s="34" t="n">
+      <c r="H25" s="19" t="n">
         <v>0.748</v>
       </c>
-      <c r="I25" s="32" t="n">
+      <c r="I25" s="17" t="n">
         <v>0.734</v>
       </c>
-      <c r="J25" s="32" t="n">
+      <c r="J25" s="17" t="n">
         <v>0.731</v>
       </c>
-      <c r="K25" s="49" t="n">
+      <c r="K25" s="32" t="n">
         <v>0.846</v>
       </c>
-      <c r="L25" s="32" t="n">
+      <c r="L25" s="17" t="n">
         <v>0.818</v>
       </c>
-      <c r="M25" s="35" t="n">
+      <c r="M25" s="16" t="n">
         <v>0.731</v>
       </c>
-      <c r="N25" s="32" t="n">
+      <c r="N25" s="17" t="n">
         <v>0.869</v>
       </c>
-      <c r="O25" s="32" t="n">
+      <c r="O25" s="17" t="n">
         <v>0.834</v>
       </c>
-      <c r="P25" s="35" t="n">
+      <c r="P25" s="16" t="n">
         <v>0.731</v>
       </c>
     </row>
@@ -1895,43 +1839,43 @@
       <c r="C26" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="36" t="n">
+      <c r="D26" s="20" t="n">
         <v>0.756</v>
       </c>
-      <c r="E26" s="36" t="n">
+      <c r="E26" s="20" t="n">
         <v>0.786</v>
       </c>
-      <c r="F26" s="36" t="n">
+      <c r="F26" s="20" t="n">
         <v>0.816</v>
       </c>
-      <c r="G26" s="37" t="n">
+      <c r="G26" s="21" t="n">
         <v>0.856</v>
       </c>
-      <c r="H26" s="38" t="n">
+      <c r="H26" s="22" t="n">
         <v>0.725</v>
       </c>
-      <c r="I26" s="36" t="n">
+      <c r="I26" s="20" t="n">
         <v>0.725</v>
       </c>
-      <c r="J26" s="36" t="n">
+      <c r="J26" s="20" t="n">
         <v>0.808</v>
       </c>
-      <c r="K26" s="38" t="n">
+      <c r="K26" s="22" t="n">
         <v>0.837</v>
       </c>
-      <c r="L26" s="36" t="n">
+      <c r="L26" s="20" t="n">
         <v>0.817</v>
       </c>
-      <c r="M26" s="39" t="n">
+      <c r="M26" s="10" t="n">
         <v>0.808</v>
       </c>
-      <c r="N26" s="36" t="n">
+      <c r="N26" s="20" t="n">
         <v>0.867</v>
       </c>
-      <c r="O26" s="36" t="n">
+      <c r="O26" s="20" t="n">
         <v>0.835</v>
       </c>
-      <c r="P26" s="39" t="n">
+      <c r="P26" s="10" t="n">
         <v>0.808</v>
       </c>
     </row>
@@ -1941,43 +1885,43 @@
       <c r="C27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="40" t="n">
+      <c r="D27" s="23" t="n">
         <v>0.789</v>
       </c>
-      <c r="E27" s="40" t="n">
+      <c r="E27" s="23" t="n">
         <v>0.772</v>
       </c>
-      <c r="F27" s="40" t="n">
+      <c r="F27" s="23" t="n">
         <v>0.829</v>
       </c>
-      <c r="G27" s="40" t="n">
+      <c r="G27" s="23" t="n">
         <v>0.831</v>
       </c>
-      <c r="H27" s="42" t="n">
+      <c r="H27" s="25" t="n">
         <v>0.772</v>
       </c>
-      <c r="I27" s="40" t="n">
+      <c r="I27" s="23" t="n">
         <v>0.744</v>
       </c>
-      <c r="J27" s="40" t="n">
+      <c r="J27" s="23" t="n">
         <v>0.667</v>
       </c>
-      <c r="K27" s="50" t="n">
+      <c r="K27" s="33" t="n">
         <v>0.854</v>
       </c>
-      <c r="L27" s="40" t="n">
+      <c r="L27" s="23" t="n">
         <v>0.819</v>
       </c>
-      <c r="M27" s="43" t="n">
+      <c r="M27" s="8" t="n">
         <v>0.667</v>
       </c>
-      <c r="N27" s="40" t="n">
+      <c r="N27" s="23" t="n">
         <v>0.87</v>
       </c>
-      <c r="O27" s="40" t="n">
+      <c r="O27" s="23" t="n">
         <v>0.834</v>
       </c>
-      <c r="P27" s="43" t="n">
+      <c r="P27" s="8" t="n">
         <v>0.667</v>
       </c>
     </row>
@@ -1989,43 +1933,43 @@
       <c r="C28" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="36" t="n">
+      <c r="D28" s="20" t="n">
         <v>0.751</v>
       </c>
-      <c r="E28" s="36" t="n">
+      <c r="E28" s="20" t="n">
         <v>0.759</v>
       </c>
-      <c r="F28" s="36" t="n">
+      <c r="F28" s="20" t="n">
         <v>0.822</v>
       </c>
-      <c r="G28" s="36" t="n">
+      <c r="G28" s="20" t="n">
         <v>0.824</v>
       </c>
-      <c r="H28" s="38" t="n">
+      <c r="H28" s="22" t="n">
         <v>0.774</v>
       </c>
-      <c r="I28" s="36" t="n">
+      <c r="I28" s="20" t="n">
         <v>0.764</v>
       </c>
-      <c r="J28" s="36" t="n">
+      <c r="J28" s="20" t="n">
         <v>0.701</v>
       </c>
-      <c r="K28" s="44" t="n">
+      <c r="K28" s="26" t="n">
         <v>0.863</v>
       </c>
-      <c r="L28" s="36" t="n">
+      <c r="L28" s="20" t="n">
         <v>0.836</v>
       </c>
-      <c r="M28" s="39" t="n">
+      <c r="M28" s="10" t="n">
         <v>0.701</v>
       </c>
-      <c r="N28" s="36" t="n">
+      <c r="N28" s="20" t="n">
         <v>0.879</v>
       </c>
-      <c r="O28" s="36" t="n">
+      <c r="O28" s="20" t="n">
         <v>0.844</v>
       </c>
-      <c r="P28" s="39" t="n">
+      <c r="P28" s="10" t="n">
         <v>0.701</v>
       </c>
     </row>
@@ -2035,43 +1979,43 @@
       <c r="C29" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="36" t="n">
+      <c r="D29" s="20" t="n">
         <v>0.787</v>
       </c>
-      <c r="E29" s="36" t="n">
+      <c r="E29" s="20" t="n">
         <v>0.806</v>
       </c>
-      <c r="F29" s="36" t="n">
+      <c r="F29" s="20" t="n">
         <v>0.821</v>
       </c>
-      <c r="G29" s="36" t="n">
+      <c r="G29" s="20" t="n">
         <v>0.847</v>
       </c>
-      <c r="H29" s="38" t="n">
+      <c r="H29" s="22" t="n">
         <v>0.763</v>
       </c>
-      <c r="I29" s="36" t="n">
+      <c r="I29" s="20" t="n">
         <v>0.769</v>
       </c>
-      <c r="J29" s="36" t="n">
+      <c r="J29" s="20" t="n">
         <v>0.839</v>
       </c>
-      <c r="K29" s="44" t="n">
+      <c r="K29" s="26" t="n">
         <v>0.867</v>
       </c>
-      <c r="L29" s="36" t="n">
+      <c r="L29" s="20" t="n">
         <v>0.843</v>
       </c>
-      <c r="M29" s="39" t="n">
+      <c r="M29" s="10" t="n">
         <v>0.839</v>
       </c>
-      <c r="N29" s="36" t="n">
+      <c r="N29" s="20" t="n">
         <v>0.888</v>
       </c>
-      <c r="O29" s="36" t="n">
+      <c r="O29" s="20" t="n">
         <v>0.852</v>
       </c>
-      <c r="P29" s="39" t="n">
+      <c r="P29" s="10" t="n">
         <v>0.839</v>
       </c>
     </row>
@@ -2081,43 +2025,43 @@
       <c r="C30" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="36" t="n">
+      <c r="D30" s="20" t="n">
         <v>0.774</v>
       </c>
-      <c r="E30" s="36" t="n">
+      <c r="E30" s="20" t="n">
         <v>0.759</v>
       </c>
-      <c r="F30" s="36" t="n">
+      <c r="F30" s="20" t="n">
         <v>0.842</v>
       </c>
-      <c r="G30" s="36" t="n">
+      <c r="G30" s="20" t="n">
         <v>0.84</v>
       </c>
-      <c r="H30" s="38" t="n">
+      <c r="H30" s="22" t="n">
         <v>0.808</v>
       </c>
-      <c r="I30" s="36" t="n">
+      <c r="I30" s="20" t="n">
         <v>0.786</v>
       </c>
-      <c r="J30" s="36" t="n">
+      <c r="J30" s="20" t="n">
         <v>0.679</v>
       </c>
-      <c r="K30" s="44" t="n">
+      <c r="K30" s="26" t="n">
         <v>0.878</v>
       </c>
-      <c r="L30" s="36" t="n">
+      <c r="L30" s="20" t="n">
         <v>0.853</v>
       </c>
-      <c r="M30" s="39" t="n">
+      <c r="M30" s="10" t="n">
         <v>0.679</v>
       </c>
-      <c r="N30" s="36" t="n">
+      <c r="N30" s="20" t="n">
         <v>0.888</v>
       </c>
-      <c r="O30" s="36" t="n">
+      <c r="O30" s="20" t="n">
         <v>0.86</v>
       </c>
-      <c r="P30" s="39" t="n">
+      <c r="P30" s="10" t="n">
         <v>0.679</v>
       </c>
     </row>
@@ -2127,43 +2071,43 @@
         <v>23</v>
       </c>
       <c r="C31" s="27"/>
-      <c r="D31" s="45" t="n">
+      <c r="D31" s="28" t="n">
         <v>0.7</v>
       </c>
-      <c r="E31" s="45" t="n">
+      <c r="E31" s="28" t="n">
         <v>2.9</v>
       </c>
-      <c r="F31" s="45" t="n">
+      <c r="F31" s="28" t="n">
         <v>105.6</v>
       </c>
-      <c r="G31" s="45" t="s">
+      <c r="G31" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="46" t="n">
+      <c r="H31" s="29" t="n">
         <v>44.7</v>
       </c>
-      <c r="I31" s="45" t="n">
+      <c r="I31" s="28" t="n">
         <v>31.9</v>
       </c>
-      <c r="J31" s="45" t="n">
+      <c r="J31" s="28" t="n">
         <v>28.3</v>
       </c>
-      <c r="K31" s="46" t="n">
+      <c r="K31" s="29" t="n">
         <v>44.1</v>
       </c>
-      <c r="L31" s="45" t="n">
+      <c r="L31" s="28" t="n">
         <v>32.1</v>
       </c>
-      <c r="M31" s="47" t="n">
+      <c r="M31" s="30" t="n">
         <v>28.2</v>
       </c>
-      <c r="N31" s="45" t="n">
+      <c r="N31" s="28" t="n">
         <v>44.3</v>
       </c>
-      <c r="O31" s="45" t="n">
+      <c r="O31" s="28" t="n">
         <v>32.2</v>
       </c>
-      <c r="P31" s="47" t="n">
+      <c r="P31" s="30" t="n">
         <v>28.4</v>
       </c>
     </row>
@@ -2177,17 +2121,17 @@
       <c r="C32" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="11" t="e">
+      <c r="D32" s="11" t="n">
         <f aca="false">ROUND(2*D35*D38/(D35+D38),3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E32" s="11" t="e">
+        <v>0.772</v>
+      </c>
+      <c r="E32" s="11" t="n">
         <f aca="false">ROUND(2*E35*E38/(E35+E38),3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F32" s="11" t="e">
+        <v>0.782</v>
+      </c>
+      <c r="F32" s="11" t="n">
         <f aca="false">ROUND(2*F35*F38/(F35+F38),3)</f>
-        <v>#DIV/0!</v>
+        <v>0.832</v>
       </c>
       <c r="G32" s="11" t="e">
         <f aca="false">ROUND(2*G35*G38/(G35+G38),3)</f>
@@ -2201,7 +2145,7 @@
         <f aca="false">ROUND(2*I35*I38/(I35+I38),3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J32" s="51" t="e">
+      <c r="J32" s="11" t="e">
         <f aca="false">ROUND(2*J35*J38/(J35+J38),3)</f>
         <v>#DIV/0!</v>
       </c>
@@ -2236,17 +2180,17 @@
       <c r="C33" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="11" t="e">
+      <c r="D33" s="11" t="n">
         <f aca="false">ROUND(2*D36*D39/(D36+D39),3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E33" s="11" t="e">
+        <v>0.768</v>
+      </c>
+      <c r="E33" s="11" t="n">
         <f aca="false">ROUND(2*E36*E39/(E36+E39),3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F33" s="11" t="e">
+        <v>0.79</v>
+      </c>
+      <c r="F33" s="11" t="n">
         <f aca="false">ROUND(2*F36*F39/(F36+F39),3)</f>
-        <v>#DIV/0!</v>
+        <v>0.815</v>
       </c>
       <c r="G33" s="11" t="e">
         <f aca="false">ROUND(2*G36*G39/(G36+G39),3)</f>
@@ -2295,17 +2239,17 @@
       <c r="C34" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="11" t="e">
+      <c r="D34" s="11" t="n">
         <f aca="false">ROUND(2*D37*D40/(D37+D40),3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E34" s="11" t="e">
+        <v>0.812</v>
+      </c>
+      <c r="E34" s="11" t="n">
         <f aca="false">ROUND(2*E37*E40/(E37+E40),3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F34" s="11" t="e">
+        <v>0.803</v>
+      </c>
+      <c r="F34" s="11" t="n">
         <f aca="false">ROUND(2*F37*F40/(F37+F40),3)</f>
-        <v>#DIV/0!</v>
+        <v>0.865</v>
       </c>
       <c r="G34" s="11" t="e">
         <f aca="false">ROUND(2*G37*G40/(G37+G40),3)</f>
@@ -2356,19 +2300,25 @@
       <c r="C35" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="52"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="54"/>
-      <c r="N35" s="52"/>
-      <c r="O35" s="52"/>
-      <c r="P35" s="54"/>
+      <c r="D35" s="34" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="E35" s="34" t="n">
+        <v>0.793</v>
+      </c>
+      <c r="F35" s="34" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="G35" s="35"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="36"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
+      <c r="P35" s="37"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8"/>
@@ -2376,19 +2326,25 @@
       <c r="C36" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="56"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="57"/>
-      <c r="N36" s="55"/>
-      <c r="O36" s="55"/>
-      <c r="P36" s="57"/>
+      <c r="D36" s="38" t="n">
+        <v>0.753</v>
+      </c>
+      <c r="E36" s="38" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="F36" s="38" t="n">
+        <v>0.814</v>
+      </c>
+      <c r="G36" s="39"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="39"/>
+      <c r="P36" s="41"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8"/>
@@ -2396,19 +2352,25 @@
       <c r="C37" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="58"/>
-      <c r="M37" s="60"/>
-      <c r="N37" s="58"/>
-      <c r="O37" s="58"/>
-      <c r="P37" s="60"/>
+      <c r="D37" s="42" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="E37" s="42" t="n">
+        <v>0.807</v>
+      </c>
+      <c r="F37" s="42" t="n">
+        <v>0.859</v>
+      </c>
+      <c r="G37" s="43"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="43"/>
+      <c r="P37" s="45"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="8"/>
@@ -2418,19 +2380,25 @@
       <c r="C38" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="56"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="57"/>
-      <c r="N38" s="55"/>
-      <c r="O38" s="55"/>
-      <c r="P38" s="57"/>
+      <c r="D38" s="38" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="E38" s="38" t="n">
+        <v>0.772</v>
+      </c>
+      <c r="F38" s="38" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="G38" s="39"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="39"/>
+      <c r="P38" s="41"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8"/>
@@ -2438,19 +2406,25 @@
       <c r="C39" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="55"/>
-      <c r="M39" s="57"/>
-      <c r="N39" s="55"/>
-      <c r="O39" s="55"/>
-      <c r="P39" s="57"/>
+      <c r="D39" s="38" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="E39" s="38" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F39" s="38" t="n">
+        <v>0.817</v>
+      </c>
+      <c r="G39" s="39"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="39"/>
+      <c r="O39" s="39"/>
+      <c r="P39" s="41"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8"/>
@@ -2458,19 +2432,25 @@
       <c r="C40" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="55"/>
-      <c r="E40" s="55"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="56"/>
-      <c r="L40" s="55"/>
-      <c r="M40" s="57"/>
-      <c r="N40" s="55"/>
-      <c r="O40" s="55"/>
-      <c r="P40" s="57"/>
+      <c r="D40" s="38" t="n">
+        <v>0.804</v>
+      </c>
+      <c r="E40" s="38" t="n">
+        <v>0.799</v>
+      </c>
+      <c r="F40" s="38" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="G40" s="39"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="39"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="39"/>
+      <c r="O40" s="39"/>
+      <c r="P40" s="41"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="8"/>
@@ -2478,19 +2458,25 @@
         <v>23</v>
       </c>
       <c r="C41" s="27"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="62"/>
-      <c r="I41" s="61"/>
-      <c r="J41" s="61"/>
-      <c r="K41" s="62"/>
-      <c r="L41" s="61"/>
-      <c r="M41" s="63"/>
-      <c r="N41" s="61"/>
-      <c r="O41" s="61"/>
-      <c r="P41" s="63"/>
+      <c r="D41" s="46" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E41" s="46" t="n">
+        <v>3</v>
+      </c>
+      <c r="F41" s="46" t="n">
+        <v>105.8</v>
+      </c>
+      <c r="G41" s="47"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="47"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="47"/>
+      <c r="O41" s="47"/>
+      <c r="P41" s="49"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
@@ -2681,19 +2667,19 @@
       <c r="C45" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="52"/>
-      <c r="E45" s="52"/>
-      <c r="F45" s="52"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="52"/>
-      <c r="M45" s="54"/>
-      <c r="N45" s="52"/>
-      <c r="O45" s="52"/>
-      <c r="P45" s="54"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="35"/>
+      <c r="O45" s="35"/>
+      <c r="P45" s="37"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8"/>
@@ -2701,19 +2687,19 @@
       <c r="C46" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="55"/>
-      <c r="K46" s="56"/>
-      <c r="L46" s="55"/>
-      <c r="M46" s="57"/>
-      <c r="N46" s="55"/>
-      <c r="O46" s="55"/>
-      <c r="P46" s="57"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="39"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="39"/>
+      <c r="O46" s="39"/>
+      <c r="P46" s="41"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8"/>
@@ -2721,19 +2707,19 @@
       <c r="C47" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
-      <c r="K47" s="59"/>
-      <c r="L47" s="58"/>
-      <c r="M47" s="60"/>
-      <c r="N47" s="58"/>
-      <c r="O47" s="58"/>
-      <c r="P47" s="60"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="45"/>
+      <c r="N47" s="43"/>
+      <c r="O47" s="43"/>
+      <c r="P47" s="45"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="8"/>
@@ -2743,19 +2729,19 @@
       <c r="C48" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="56"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="56"/>
-      <c r="L48" s="55"/>
-      <c r="M48" s="57"/>
-      <c r="N48" s="55"/>
-      <c r="O48" s="55"/>
-      <c r="P48" s="57"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="39"/>
+      <c r="K48" s="40"/>
+      <c r="L48" s="39"/>
+      <c r="M48" s="41"/>
+      <c r="N48" s="39"/>
+      <c r="O48" s="39"/>
+      <c r="P48" s="41"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8"/>
@@ -2763,19 +2749,19 @@
       <c r="C49" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="55"/>
-      <c r="H49" s="56"/>
-      <c r="I49" s="55"/>
-      <c r="J49" s="55"/>
-      <c r="K49" s="56"/>
-      <c r="L49" s="55"/>
-      <c r="M49" s="57"/>
-      <c r="N49" s="55"/>
-      <c r="O49" s="55"/>
-      <c r="P49" s="57"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="39"/>
+      <c r="M49" s="41"/>
+      <c r="N49" s="39"/>
+      <c r="O49" s="39"/>
+      <c r="P49" s="41"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8"/>
@@ -2783,19 +2769,19 @@
       <c r="C50" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="55"/>
-      <c r="E50" s="55"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="55"/>
-      <c r="H50" s="56"/>
-      <c r="I50" s="55"/>
-      <c r="J50" s="55"/>
-      <c r="K50" s="56"/>
-      <c r="L50" s="55"/>
-      <c r="M50" s="57"/>
-      <c r="N50" s="55"/>
-      <c r="O50" s="55"/>
-      <c r="P50" s="57"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="40"/>
+      <c r="L50" s="39"/>
+      <c r="M50" s="41"/>
+      <c r="N50" s="39"/>
+      <c r="O50" s="39"/>
+      <c r="P50" s="41"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="8"/>
@@ -2803,19 +2789,19 @@
         <v>23</v>
       </c>
       <c r="C51" s="27"/>
-      <c r="D51" s="61"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
-      <c r="H51" s="62"/>
-      <c r="I51" s="61"/>
-      <c r="J51" s="61"/>
-      <c r="K51" s="62"/>
-      <c r="L51" s="61"/>
-      <c r="M51" s="63"/>
-      <c r="N51" s="61"/>
-      <c r="O51" s="61"/>
-      <c r="P51" s="63"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="47"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="47"/>
+      <c r="J51" s="47"/>
+      <c r="K51" s="48"/>
+      <c r="L51" s="47"/>
+      <c r="M51" s="49"/>
+      <c r="N51" s="47"/>
+      <c r="O51" s="47"/>
+      <c r="P51" s="49"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="s">
@@ -3006,19 +2992,19 @@
       <c r="C55" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D55" s="52"/>
-      <c r="E55" s="52"/>
-      <c r="F55" s="52"/>
-      <c r="G55" s="52"/>
-      <c r="H55" s="53"/>
-      <c r="I55" s="52"/>
-      <c r="J55" s="52"/>
-      <c r="K55" s="53"/>
-      <c r="L55" s="52"/>
-      <c r="M55" s="54"/>
-      <c r="N55" s="52"/>
-      <c r="O55" s="52"/>
-      <c r="P55" s="54"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="36"/>
+      <c r="L55" s="35"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="35"/>
+      <c r="O55" s="35"/>
+      <c r="P55" s="37"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8"/>
@@ -3026,19 +3012,19 @@
       <c r="C56" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D56" s="55"/>
-      <c r="E56" s="55"/>
-      <c r="F56" s="55"/>
-      <c r="G56" s="55"/>
-      <c r="H56" s="56"/>
-      <c r="I56" s="55"/>
-      <c r="J56" s="55"/>
-      <c r="K56" s="56"/>
-      <c r="L56" s="55"/>
-      <c r="M56" s="57"/>
-      <c r="N56" s="55"/>
-      <c r="O56" s="55"/>
-      <c r="P56" s="57"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="40"/>
+      <c r="L56" s="39"/>
+      <c r="M56" s="41"/>
+      <c r="N56" s="39"/>
+      <c r="O56" s="39"/>
+      <c r="P56" s="41"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8"/>
@@ -3046,19 +3032,19 @@
       <c r="C57" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="59"/>
-      <c r="I57" s="58"/>
-      <c r="J57" s="58"/>
-      <c r="K57" s="59"/>
-      <c r="L57" s="58"/>
-      <c r="M57" s="60"/>
-      <c r="N57" s="58"/>
-      <c r="O57" s="58"/>
-      <c r="P57" s="60"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="44"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="44"/>
+      <c r="L57" s="43"/>
+      <c r="M57" s="45"/>
+      <c r="N57" s="43"/>
+      <c r="O57" s="43"/>
+      <c r="P57" s="45"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="8"/>
@@ -3068,19 +3054,19 @@
       <c r="C58" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D58" s="55"/>
-      <c r="E58" s="55"/>
-      <c r="F58" s="55"/>
-      <c r="G58" s="55"/>
-      <c r="H58" s="56"/>
-      <c r="I58" s="55"/>
-      <c r="J58" s="55"/>
-      <c r="K58" s="56"/>
-      <c r="L58" s="55"/>
-      <c r="M58" s="57"/>
-      <c r="N58" s="55"/>
-      <c r="O58" s="55"/>
-      <c r="P58" s="57"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="39"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="40"/>
+      <c r="L58" s="39"/>
+      <c r="M58" s="41"/>
+      <c r="N58" s="39"/>
+      <c r="O58" s="39"/>
+      <c r="P58" s="41"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8"/>
@@ -3088,19 +3074,19 @@
       <c r="C59" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="55"/>
-      <c r="H59" s="56"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="55"/>
-      <c r="K59" s="56"/>
-      <c r="L59" s="55"/>
-      <c r="M59" s="57"/>
-      <c r="N59" s="55"/>
-      <c r="O59" s="55"/>
-      <c r="P59" s="57"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="39"/>
+      <c r="J59" s="39"/>
+      <c r="K59" s="40"/>
+      <c r="L59" s="39"/>
+      <c r="M59" s="41"/>
+      <c r="N59" s="39"/>
+      <c r="O59" s="39"/>
+      <c r="P59" s="41"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8"/>
@@ -3108,19 +3094,19 @@
       <c r="C60" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D60" s="55"/>
-      <c r="E60" s="55"/>
-      <c r="F60" s="55"/>
-      <c r="G60" s="55"/>
-      <c r="H60" s="56"/>
-      <c r="I60" s="55"/>
-      <c r="J60" s="55"/>
-      <c r="K60" s="56"/>
-      <c r="L60" s="55"/>
-      <c r="M60" s="57"/>
-      <c r="N60" s="55"/>
-      <c r="O60" s="55"/>
-      <c r="P60" s="57"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="40"/>
+      <c r="I60" s="39"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="40"/>
+      <c r="L60" s="39"/>
+      <c r="M60" s="41"/>
+      <c r="N60" s="39"/>
+      <c r="O60" s="39"/>
+      <c r="P60" s="41"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="8"/>
@@ -3128,19 +3114,19 @@
         <v>23</v>
       </c>
       <c r="C61" s="27"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="61"/>
-      <c r="G61" s="61"/>
-      <c r="H61" s="62"/>
-      <c r="I61" s="61"/>
-      <c r="J61" s="61"/>
-      <c r="K61" s="62"/>
-      <c r="L61" s="61"/>
-      <c r="M61" s="63"/>
-      <c r="N61" s="61"/>
-      <c r="O61" s="61"/>
-      <c r="P61" s="63"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="48"/>
+      <c r="L61" s="47"/>
+      <c r="M61" s="49"/>
+      <c r="N61" s="47"/>
+      <c r="O61" s="47"/>
+      <c r="P61" s="49"/>
     </row>
     <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">

</xml_diff>

<commit_message>
t-test p-values for single-sequence
</commit_message>
<xml_diff>
--- a/benchmarks/summary.xlsx
+++ b/benchmarks/summary.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="short table" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="p-values" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="57">
   <si>
     <t xml:space="preserve">Dataset</t>
   </si>
@@ -227,16 +228,23 @@
   <si>
     <t xml:space="preserve">Harmonized</t>
   </si>
+  <si>
+    <t xml:space="preserve">Pairwise t-test p-values on SRtrain dataset results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pairwise t-test p-values on TS1reducedWC dataset results</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -273,6 +281,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -282,7 +297,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -367,6 +382,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -393,7 +415,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -534,12 +556,36 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3765,8 +3811,8 @@
   </sheetPr>
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3775,38 +3821,38 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="5" t="s">
         <v>50</v>
       </c>
@@ -3821,212 +3867,212 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="35" t="n">
+      <c r="C3" s="36" t="n">
         <v>0.723</v>
       </c>
-      <c r="D3" s="35" t="n">
+      <c r="D3" s="36" t="n">
         <v>0.742</v>
       </c>
-      <c r="E3" s="35" t="n">
+      <c r="E3" s="36" t="n">
         <v>0.793</v>
       </c>
-      <c r="F3" s="36" t="n">
+      <c r="F3" s="37" t="n">
         <v>0.819</v>
       </c>
-      <c r="G3" s="35" t="n">
+      <c r="G3" s="36" t="n">
         <v>0.721</v>
       </c>
-      <c r="H3" s="35" t="n">
+      <c r="H3" s="36" t="n">
         <v>0.715</v>
       </c>
-      <c r="I3" s="35" t="n">
+      <c r="I3" s="36" t="n">
         <v>0.788</v>
       </c>
-      <c r="J3" s="35" t="n">
+      <c r="J3" s="36" t="n">
         <v>0.766</v>
       </c>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="35" t="n">
+      <c r="C4" s="36" t="n">
         <v>0.721</v>
       </c>
-      <c r="D4" s="35" t="n">
+      <c r="D4" s="36" t="n">
         <v>0.743</v>
       </c>
-      <c r="E4" s="35" t="n">
+      <c r="E4" s="36" t="n">
         <v>0.795</v>
       </c>
-      <c r="F4" s="36" t="n">
+      <c r="F4" s="37" t="n">
         <v>0.82</v>
       </c>
-      <c r="G4" s="35" t="n">
+      <c r="G4" s="36" t="n">
         <v>0.72</v>
       </c>
-      <c r="H4" s="35" t="n">
+      <c r="H4" s="36" t="n">
         <v>0.712</v>
       </c>
-      <c r="I4" s="35" t="n">
+      <c r="I4" s="36" t="n">
         <v>0.778</v>
       </c>
-      <c r="J4" s="35" t="n">
+      <c r="J4" s="36" t="n">
         <v>0.757</v>
       </c>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="35" t="n">
+      <c r="C5" s="36" t="n">
         <v>0.725</v>
       </c>
-      <c r="D5" s="35" t="n">
+      <c r="D5" s="36" t="n">
         <v>0.742</v>
       </c>
-      <c r="E5" s="35" t="n">
+      <c r="E5" s="36" t="n">
         <v>0.792</v>
       </c>
-      <c r="F5" s="36" t="n">
+      <c r="F5" s="37" t="n">
         <v>0.819</v>
       </c>
-      <c r="G5" s="35" t="n">
+      <c r="G5" s="36" t="n">
         <v>0.722</v>
       </c>
-      <c r="H5" s="35" t="n">
+      <c r="H5" s="36" t="n">
         <v>0.718</v>
       </c>
-      <c r="I5" s="35" t="n">
+      <c r="I5" s="36" t="n">
         <v>0.799</v>
       </c>
-      <c r="J5" s="35" t="n">
+      <c r="J5" s="36" t="n">
         <v>0.776</v>
       </c>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="36"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="35" t="n">
+      <c r="C6" s="36" t="n">
         <v>0.72</v>
       </c>
-      <c r="D6" s="35" t="n">
+      <c r="D6" s="36" t="n">
         <v>0.751</v>
       </c>
-      <c r="E6" s="36" t="n">
+      <c r="E6" s="37" t="n">
         <v>0.789</v>
       </c>
-      <c r="F6" s="35" t="n">
+      <c r="F6" s="36" t="n">
         <v>0.774</v>
       </c>
-      <c r="G6" s="35" t="n">
+      <c r="G6" s="36" t="n">
         <v>0.702</v>
       </c>
-      <c r="H6" s="35" t="n">
+      <c r="H6" s="36" t="n">
         <v>0.691</v>
       </c>
-      <c r="I6" s="35" t="n">
+      <c r="I6" s="36" t="n">
         <v>0.777</v>
       </c>
-      <c r="J6" s="35" t="n">
+      <c r="J6" s="36" t="n">
         <v>0.754</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="35" t="n">
+      <c r="C7" s="36" t="n">
         <v>0.694</v>
       </c>
-      <c r="D7" s="35" t="n">
+      <c r="D7" s="36" t="n">
         <v>0.746</v>
       </c>
-      <c r="E7" s="36" t="n">
+      <c r="E7" s="37" t="n">
         <v>0.762</v>
       </c>
-      <c r="F7" s="35" t="n">
+      <c r="F7" s="36" t="n">
         <v>0.734</v>
       </c>
-      <c r="G7" s="35" t="n">
+      <c r="G7" s="36" t="n">
         <v>0.648</v>
       </c>
-      <c r="H7" s="35" t="n">
+      <c r="H7" s="36" t="n">
         <v>0.636</v>
       </c>
-      <c r="I7" s="35" t="n">
+      <c r="I7" s="36" t="n">
         <v>0.713</v>
       </c>
-      <c r="J7" s="35" t="n">
+      <c r="J7" s="36" t="n">
         <v>0.693</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="35" t="n">
+      <c r="C8" s="36" t="n">
         <v>0.748</v>
       </c>
-      <c r="D8" s="35" t="n">
+      <c r="D8" s="36" t="n">
         <v>0.757</v>
       </c>
-      <c r="E8" s="35" t="n">
+      <c r="E8" s="36" t="n">
         <v>0.819</v>
       </c>
-      <c r="F8" s="35" t="n">
+      <c r="F8" s="36" t="n">
         <v>0.818</v>
       </c>
-      <c r="G8" s="35" t="n">
+      <c r="G8" s="36" t="n">
         <v>0.767</v>
       </c>
-      <c r="H8" s="35" t="n">
+      <c r="H8" s="36" t="n">
         <v>0.757</v>
       </c>
-      <c r="I8" s="36" t="n">
+      <c r="I8" s="37" t="n">
         <v>0.853</v>
       </c>
-      <c r="J8" s="35" t="n">
+      <c r="J8" s="36" t="n">
         <v>0.826</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4048,4 +4094,594 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:I27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="14.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="13.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="15.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="10" style="6" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="41" t="n">
+        <v>0.714748633931574</v>
+      </c>
+      <c r="D4" s="41" t="n">
+        <v>0.470622079632895</v>
+      </c>
+      <c r="E4" s="41" t="n">
+        <v>0.739369847846124</v>
+      </c>
+      <c r="F4" s="42" t="n">
+        <v>0.00323966900068798</v>
+      </c>
+      <c r="G4" s="42" t="n">
+        <v>0.00427870901149946</v>
+      </c>
+      <c r="H4" s="42" t="n">
+        <v>4.61842320188265E-006</v>
+      </c>
+      <c r="I4" s="42" t="n">
+        <v>0.00127716563423969</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="41" t="n">
+        <v>0.714748633931574</v>
+      </c>
+      <c r="C5" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="41" t="n">
+        <v>0.698796200466445</v>
+      </c>
+      <c r="E5" s="41" t="n">
+        <v>0.979900722810106</v>
+      </c>
+      <c r="F5" s="42" t="n">
+        <v>0.00510172041114741</v>
+      </c>
+      <c r="G5" s="42" t="n">
+        <v>0.00684192709300344</v>
+      </c>
+      <c r="H5" s="42" t="n">
+        <v>3.80211435515961E-006</v>
+      </c>
+      <c r="I5" s="42" t="n">
+        <v>0.00191276006023002</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="41" t="n">
+        <v>0.470622079632895</v>
+      </c>
+      <c r="C6" s="41" t="n">
+        <v>0.698796200466445</v>
+      </c>
+      <c r="D6" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="41" t="n">
+        <v>0.688802151948145</v>
+      </c>
+      <c r="F6" s="41" t="n">
+        <v>0.0172442449691595</v>
+      </c>
+      <c r="G6" s="41" t="n">
+        <v>0.0220691745624745</v>
+      </c>
+      <c r="H6" s="42" t="n">
+        <v>3.07472867189051E-005</v>
+      </c>
+      <c r="I6" s="42" t="n">
+        <v>0.00727308689775976</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="41" t="n">
+        <v>0.739369847846124</v>
+      </c>
+      <c r="C7" s="41" t="n">
+        <v>0.979900722810106</v>
+      </c>
+      <c r="D7" s="41" t="n">
+        <v>0.688802151948145</v>
+      </c>
+      <c r="E7" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="42" t="n">
+        <v>0.00626367984104423</v>
+      </c>
+      <c r="G7" s="42" t="n">
+        <v>0.0082428354717902</v>
+      </c>
+      <c r="H7" s="42" t="n">
+        <v>7.63745869220172E-006</v>
+      </c>
+      <c r="I7" s="42" t="n">
+        <v>0.00247253903862242</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="42" t="n">
+        <v>0.00323966900068798</v>
+      </c>
+      <c r="C8" s="42" t="n">
+        <v>0.00510172041114741</v>
+      </c>
+      <c r="D8" s="41" t="n">
+        <v>0.0172442449691595</v>
+      </c>
+      <c r="E8" s="42" t="n">
+        <v>0.00626367984104423</v>
+      </c>
+      <c r="F8" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="41" t="n">
+        <v>0.937785636744972</v>
+      </c>
+      <c r="H8" s="41" t="n">
+        <v>0.0770149786796826</v>
+      </c>
+      <c r="I8" s="41" t="n">
+        <v>0.742740723410938</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="42" t="n">
+        <v>0.00427870901149946</v>
+      </c>
+      <c r="C9" s="42" t="n">
+        <v>0.00684192709300344</v>
+      </c>
+      <c r="D9" s="41" t="n">
+        <v>0.0220691745624745</v>
+      </c>
+      <c r="E9" s="42" t="n">
+        <v>0.0082428354717902</v>
+      </c>
+      <c r="F9" s="41" t="n">
+        <v>0.937785636744972</v>
+      </c>
+      <c r="G9" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="41" t="n">
+        <v>0.0668455026641247</v>
+      </c>
+      <c r="I9" s="41" t="n">
+        <v>0.686890288395913</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="42" t="n">
+        <v>4.61842320188265E-006</v>
+      </c>
+      <c r="C10" s="42" t="n">
+        <v>3.80211435515961E-006</v>
+      </c>
+      <c r="D10" s="42" t="n">
+        <v>3.07472867189051E-005</v>
+      </c>
+      <c r="E10" s="42" t="n">
+        <v>7.63745869220172E-006</v>
+      </c>
+      <c r="F10" s="41" t="n">
+        <v>0.0770149786796826</v>
+      </c>
+      <c r="G10" s="41" t="n">
+        <v>0.0668455026641247</v>
+      </c>
+      <c r="H10" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="41" t="n">
+        <v>0.158124363498487</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="42" t="n">
+        <v>0.00127716563423969</v>
+      </c>
+      <c r="C11" s="42" t="n">
+        <v>0.00191276006023002</v>
+      </c>
+      <c r="D11" s="42" t="n">
+        <v>0.00727308689775976</v>
+      </c>
+      <c r="E11" s="42" t="n">
+        <v>0.00247253903862242</v>
+      </c>
+      <c r="F11" s="41" t="n">
+        <v>0.742740723410938</v>
+      </c>
+      <c r="G11" s="41" t="n">
+        <v>0.686890288395913</v>
+      </c>
+      <c r="H11" s="41" t="n">
+        <v>0.158124363498487</v>
+      </c>
+      <c r="I11" s="41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="41" t="n">
+        <v>0.711411801097545</v>
+      </c>
+      <c r="D15" s="41" t="n">
+        <v>0.94645508876273</v>
+      </c>
+      <c r="E15" s="41" t="n">
+        <v>0.888199908317778</v>
+      </c>
+      <c r="F15" s="41" t="n">
+        <v>0.133534414972666</v>
+      </c>
+      <c r="G15" s="41" t="n">
+        <v>0.0247248784644662</v>
+      </c>
+      <c r="H15" s="41" t="n">
+        <v>0.0967586366600864</v>
+      </c>
+      <c r="I15" s="41" t="n">
+        <v>0.262519886542744</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="41" t="n">
+        <v>0.711411801097545</v>
+      </c>
+      <c r="C16" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="41" t="n">
+        <v>0.643551513045951</v>
+      </c>
+      <c r="E16" s="41" t="n">
+        <v>0.583751662512394</v>
+      </c>
+      <c r="F16" s="41" t="n">
+        <v>0.203031022405904</v>
+      </c>
+      <c r="G16" s="41" t="n">
+        <v>0.0320950448749731</v>
+      </c>
+      <c r="H16" s="41" t="n">
+        <v>0.145243520078722</v>
+      </c>
+      <c r="I16" s="41" t="n">
+        <v>0.400100202686706</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="41" t="n">
+        <v>0.94645508876273</v>
+      </c>
+      <c r="C17" s="41" t="n">
+        <v>0.643551513045951</v>
+      </c>
+      <c r="D17" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="41" t="n">
+        <v>0.93927035337389</v>
+      </c>
+      <c r="F17" s="41" t="n">
+        <v>0.0973028474314747</v>
+      </c>
+      <c r="G17" s="41" t="n">
+        <v>0.0135961334786735</v>
+      </c>
+      <c r="H17" s="41" t="n">
+        <v>0.06728176650753</v>
+      </c>
+      <c r="I17" s="41" t="n">
+        <v>0.209396404306357</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="41" t="n">
+        <v>0.888199908317778</v>
+      </c>
+      <c r="C18" s="41" t="n">
+        <v>0.583751662512394</v>
+      </c>
+      <c r="D18" s="41" t="n">
+        <v>0.93927035337389</v>
+      </c>
+      <c r="E18" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="41" t="n">
+        <v>0.0787234319222526</v>
+      </c>
+      <c r="G18" s="42" t="n">
+        <v>0.00972895209524133</v>
+      </c>
+      <c r="H18" s="41" t="n">
+        <v>0.0532748380264439</v>
+      </c>
+      <c r="I18" s="41" t="n">
+        <v>0.176985921688705</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="41" t="n">
+        <v>0.133534414972666</v>
+      </c>
+      <c r="C19" s="41" t="n">
+        <v>0.203031022405904</v>
+      </c>
+      <c r="D19" s="41" t="n">
+        <v>0.0973028474314747</v>
+      </c>
+      <c r="E19" s="41" t="n">
+        <v>0.0787234319222526</v>
+      </c>
+      <c r="F19" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="41" t="n">
+        <v>0.415095566094501</v>
+      </c>
+      <c r="H19" s="41" t="n">
+        <v>0.858328908741505</v>
+      </c>
+      <c r="I19" s="41" t="n">
+        <v>0.664163814926686</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="41" t="n">
+        <v>0.0247248784644662</v>
+      </c>
+      <c r="C20" s="41" t="n">
+        <v>0.0320950448749731</v>
+      </c>
+      <c r="D20" s="41" t="n">
+        <v>0.0135961334786735</v>
+      </c>
+      <c r="E20" s="42" t="n">
+        <v>0.00972895209524133</v>
+      </c>
+      <c r="F20" s="41" t="n">
+        <v>0.415095566094501</v>
+      </c>
+      <c r="G20" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="41" t="n">
+        <v>0.527524598653662</v>
+      </c>
+      <c r="I20" s="41" t="n">
+        <v>0.203293307031256</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="41" t="n">
+        <v>0.0967586366600864</v>
+      </c>
+      <c r="C21" s="41" t="n">
+        <v>0.145243520078722</v>
+      </c>
+      <c r="D21" s="41" t="n">
+        <v>0.06728176650753</v>
+      </c>
+      <c r="E21" s="41" t="n">
+        <v>0.0532748380264439</v>
+      </c>
+      <c r="F21" s="41" t="n">
+        <v>0.858328908741505</v>
+      </c>
+      <c r="G21" s="41" t="n">
+        <v>0.527524598653662</v>
+      </c>
+      <c r="H21" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="41" t="n">
+        <v>0.538559748965505</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="41" t="n">
+        <v>0.262519886542744</v>
+      </c>
+      <c r="C22" s="41" t="n">
+        <v>0.400100202686706</v>
+      </c>
+      <c r="D22" s="41" t="n">
+        <v>0.209396404306357</v>
+      </c>
+      <c r="E22" s="41" t="n">
+        <v>0.176985921688705</v>
+      </c>
+      <c r="F22" s="41" t="n">
+        <v>0.664163814926686</v>
+      </c>
+      <c r="G22" s="41" t="n">
+        <v>0.203293307031256</v>
+      </c>
+      <c r="H22" s="41" t="n">
+        <v>0.538559748965505</v>
+      </c>
+      <c r="I22" s="41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A13:I13"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>